<commit_message>
Split up data from IPEDs
</commit_message>
<xml_diff>
--- a/Data/COA_Research.xlsx
+++ b/Data/COA_Research.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregchick/Desktop/Dissertation/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B655427-F188-014B-8768-FD5417047104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E1010C-F29B-E04B-BAE7-48E5B7706938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17320" windowHeight="16940" xr2:uid="{9FBBFF36-6EC8-0349-B0EA-21F8EC6A0D9B}"/>
+    <workbookView xWindow="18320" yWindow="-21100" windowWidth="15020" windowHeight="21100" xr2:uid="{9FBBFF36-6EC8-0349-B0EA-21F8EC6A0D9B}"/>
   </bookViews>
   <sheets>
     <sheet name="COA_Scholarship" sheetId="1" r:id="rId1"/>
-    <sheet name="Conference_Division_Changes" sheetId="2" r:id="rId2"/>
+    <sheet name="Changes" sheetId="2" r:id="rId2"/>
+    <sheet name="Conferences" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">COA_Scholarship!$A$1:$K$66</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="436">
   <si>
     <t>Data</t>
   </si>
@@ -1193,13 +1194,169 @@
   </si>
   <si>
     <t>Mountain West -&gt; Pac-12</t>
+  </si>
+  <si>
+    <t>Division I</t>
+  </si>
+  <si>
+    <t>Power 5</t>
+  </si>
+  <si>
+    <t>Big 12 Conference</t>
+  </si>
+  <si>
+    <t>Pac-12 Conference</t>
+  </si>
+  <si>
+    <t>Group of Five</t>
+  </si>
+  <si>
+    <t>FBS</t>
+  </si>
+  <si>
+    <t>FCS</t>
+  </si>
+  <si>
+    <t>Ivy League</t>
+  </si>
+  <si>
+    <t>Missouri Valley Football Conference</t>
+  </si>
+  <si>
+    <t>Ohio Valley Conference</t>
+  </si>
+  <si>
+    <t>Patriot League</t>
+  </si>
+  <si>
+    <t>Southwestern Athletic Conference</t>
+  </si>
+  <si>
+    <t>Nickname</t>
+  </si>
+  <si>
+    <t>MVFC</t>
+  </si>
+  <si>
+    <t>NEC</t>
+  </si>
+  <si>
+    <t>OVC</t>
+  </si>
+  <si>
+    <t>PFL</t>
+  </si>
+  <si>
+    <t>SoCon</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>Big Ten</t>
+  </si>
+  <si>
+    <t>Big 12</t>
+  </si>
+  <si>
+    <t>Pac-12</t>
+  </si>
+  <si>
+    <t>SEC</t>
+  </si>
+  <si>
+    <t>The American</t>
+  </si>
+  <si>
+    <t>C-USA</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>Sun Belt</t>
+  </si>
+  <si>
+    <t>Division II</t>
+  </si>
+  <si>
+    <t>California Collegiate Athletic Association</t>
+  </si>
+  <si>
+    <t>Central Atlantic Collegiate Conference</t>
+  </si>
+  <si>
+    <t>Central Intercollegiate Athletic Association</t>
+  </si>
+  <si>
+    <t>Conference Carolinas</t>
+  </si>
+  <si>
+    <t>East Coast Conference</t>
+  </si>
+  <si>
+    <t>Great American Conference</t>
+  </si>
+  <si>
+    <t>Great Lakes Intercollegiate Athletic Conference</t>
+  </si>
+  <si>
+    <t>Great Lakes Valley Conference</t>
+  </si>
+  <si>
+    <t>Great Midwest Athletic Conference</t>
+  </si>
+  <si>
+    <t>Great Northwest Athletic Conference</t>
+  </si>
+  <si>
+    <t>Gulf South Conference</t>
+  </si>
+  <si>
+    <t>Lone Star Conference</t>
+  </si>
+  <si>
+    <t>Mid-America Intercollegiate Athletics Association</t>
+  </si>
+  <si>
+    <t>Mountain East Conference</t>
+  </si>
+  <si>
+    <t>Northeast-10 Conference</t>
+  </si>
+  <si>
+    <t>Northern Sun Intercollegiate Conference</t>
+  </si>
+  <si>
+    <t>Pacific West Conference</t>
+  </si>
+  <si>
+    <t>Peach Belt Conference</t>
+  </si>
+  <si>
+    <t>Pennsylvania State Athletic Conference</t>
+  </si>
+  <si>
+    <t>Rocky Mountain Athletic Conference</t>
+  </si>
+  <si>
+    <t>South Atlantic Conference</t>
+  </si>
+  <si>
+    <t>Southern Intercollegiate Athletic Conference</t>
+  </si>
+  <si>
+    <t>Sunshine State Conference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1214,8 +1371,32 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1226,6 +1407,24 @@
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
         <bgColor indexed="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1256,7 +1455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1264,6 +1463,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1581,8 +1786,8 @@
   <dimension ref="A1:L189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4119,16 +4324,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0D9B67-F931-AC4F-8B59-CC52BE3B18E2}">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" zoomScale="86" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" customWidth="1"/>
-    <col min="3" max="3" width="6.5" customWidth="1"/>
-    <col min="5" max="5" width="78.83203125" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -4157,7 +4366,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>232557</v>
       </c>
@@ -4677,7 +4886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>199139</v>
       </c>
@@ -4720,7 +4929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>100663</v>
       </c>
@@ -6689,6 +6898,386 @@
       <c r="H99">
         <v>0</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24EC4B6-A72A-6F4D-8AD0-6C81EB27A750}">
+  <dimension ref="A1:B57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A30" zoomScale="131" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="10" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="10" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B57" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>